<commit_message>
Added Delete All Contact Logic
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCRMTestData.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24201"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6453808E-AC6F-4AEF-9D3C-1CFD0ED854FB}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F51A7E7-E498-4517-8191-4E0D2F4DAB74}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Firstname</t>
   </si>
@@ -62,6 +62,42 @@
   </si>
   <si>
     <t>Ebay</t>
+  </si>
+  <si>
+    <t>Varsha</t>
+  </si>
+  <si>
+    <t>Singhal</t>
+  </si>
+  <si>
+    <t>MindTree</t>
+  </si>
+  <si>
+    <t>Nidhi</t>
+  </si>
+  <si>
+    <t>Choudhary</t>
+  </si>
+  <si>
+    <t>Infosys</t>
+  </si>
+  <si>
+    <t>Upasana</t>
+  </si>
+  <si>
+    <t>Sinha</t>
+  </si>
+  <si>
+    <t>Cognizant</t>
+  </si>
+  <si>
+    <t>Ruchita</t>
+  </si>
+  <si>
+    <t>Kadam</t>
+  </si>
+  <si>
+    <t>IBM</t>
   </si>
 </sst>
 </file>
@@ -413,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -465,6 +501,50 @@
         <v>11</v>
       </c>
     </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>